<commit_message>
I have added the id generator function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,92 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NodeJS\excelWithExpress\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECDC63F-43C5-480C-8629-D8019C4FD0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>profession</t>
-  </si>
-  <si>
-    <t>course</t>
-  </si>
-  <si>
-    <t>division</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Jolisha</t>
-  </si>
-  <si>
-    <t>Professor</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>CSE</t>
-  </si>
-  <si>
-    <t>Software Developer</t>
-  </si>
-  <si>
-    <t>Adlin Jelsia</t>
-  </si>
-  <si>
-    <t>Teacher</t>
-  </si>
-  <si>
-    <t>BSC</t>
-  </si>
-  <si>
-    <t>Maths</t>
-  </si>
-  <si>
-    <t>Raja</t>
-  </si>
-  <si>
-    <t>ECE</t>
-  </si>
-  <si>
-    <t>Prince</t>
-  </si>
-  <si>
-    <t>EEE</t>
-  </si>
-  <si>
-    <t>angelin</t>
-  </si>
-  <si>
-    <t>Server Manager</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -455,127 +396,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
-    <col min="3" max="3" width="19.4375" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>profession</v>
+      </c>
+      <c r="C1" t="str">
+        <v>course</v>
+      </c>
+      <c r="D1" t="str">
+        <v>division</v>
+      </c>
+      <c r="E1" t="str">
+        <v>id</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Jolisha</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Professor</v>
+      </c>
+      <c r="C2" t="str">
+        <v>BE</v>
+      </c>
+      <c r="D2" t="str">
+        <v>CSE</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Prince</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Software Developer</v>
+      </c>
+      <c r="C3" t="str">
+        <v>BE</v>
+      </c>
+      <c r="D3" t="str">
+        <v>EEE</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Adlin Jelsia</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Teacher</v>
+      </c>
+      <c r="C4" t="str">
+        <v>BSC</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Maths</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Raja</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Software Developer</v>
+      </c>
+      <c r="C5" t="str">
+        <v>BE</v>
+      </c>
+      <c r="D5" t="str">
+        <v>ECE</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>angelin</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Server Manager</v>
+      </c>
+      <c r="C6" t="str">
+        <v>BSC</v>
+      </c>
+      <c r="D6" t="str">
+        <v>CSE</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Sherlin</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Doctor</v>
+      </c>
+      <c r="C7" t="str">
+        <v>MBBS</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Nurology</v>
+      </c>
+      <c r="E7">
+        <v>114687992</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Sathya</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Collector</v>
+      </c>
+      <c r="C8" t="str">
+        <v>BE</v>
+      </c>
+      <c r="D8" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="E8">
+        <v>936993069</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:E2 A5:D5 A4:E4 B3:C3 E3 A1:D1" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>